<commit_message>
updated everything to match readme
</commit_message>
<xml_diff>
--- a/Extended Markdown Application Support.xlsx
+++ b/Extended Markdown Application Support.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Code in fenced block</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Heading with id attribute</t>
   </si>
   <si>
-    <t>HTML in raw form</t>
-  </si>
-  <si>
     <t>Link auto (disabled)</t>
   </si>
   <si>
@@ -65,14 +62,32 @@
     <t>Link auto</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
+    <t>Notepad++ with MarkdownViewer++ extension</t>
+  </si>
+  <si>
+    <t>Visual Studio Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yes
-Filters out the following tags: 
+</t>
+  </si>
+  <si>
+    <t>Yes, but doesn’t support the shortcode.</t>
+  </si>
+  <si>
+    <t>HTML inline</t>
+  </si>
+  <si>
+    <t>Yes.</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Yes. Filters out these elements: 
 &lt;title&gt;
 &lt;textarea&gt;
 &lt;style&gt;
@@ -81,32 +96,18 @@
 &lt;noembed&gt;
 &lt;noframes&gt;
 &lt;script&gt;
-&lt;plaintext&gt;
-</t>
-  </si>
-  <si>
-    <t>Notepad++ with MarkdownViewer++ extension</t>
-  </si>
-  <si>
-    <t>Visual Studio Code</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes
-</t>
-  </si>
-  <si>
-    <t>No
+&lt;plaintext&gt;</t>
+  </si>
+  <si>
+    <t>No.
 View shows nothing, but generated HTML shows emoji that was copied and pasted.</t>
-  </si>
-  <si>
-    <t>Yes, but doesn’t support the shortcode.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +119,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,26 +153,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -171,7 +194,14 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF92D050"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
         </patternFill>
       </fill>
     </dxf>
@@ -182,12 +212,157 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF6FE38D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
         </patternFill>
       </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC6EFCE"/>
+      <color rgb="FFFF9999"/>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FF6FE38D"/>
+      <color rgb="FFA2E6B4"/>
+      <color rgb="FF00BC3A"/>
+      <color rgb="FF9CE4BE"/>
+      <color rgb="FF50D08D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -462,205 +637,245 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.7109375" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="225" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D13">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:L13">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="No.">
+      <formula>NOT(ISERROR(SEARCH("No.",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId2"/>
+    <hyperlink ref="D1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>